<commit_message>
Hide setting kanan,cek import, menu
</commit_message>
<xml_diff>
--- a/public/dataimportpegawai.xlsx
+++ b/public/dataimportpegawai.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PRG\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGGAPUR\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{99D9B59F-C87F-4924-B459-AFE370105E26}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59711753-7910-4311-A86E-5B6E4135E2E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{E6091B60-0E80-4353-BB3B-59A1F9DF82B5}"/>
   </bookViews>
@@ -94,9 +94,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$Rp-421]#,##0"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,13 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15CC9845-81BD-403A-8B59-96004B4E43DC}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AI104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +454,11 @@
     <col min="6" max="6" width="20.140625" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" customWidth="1"/>
     <col min="11" max="11" width="21.140625" customWidth="1"/>
+    <col min="12" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -528,246 +527,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="U2" s="3"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="U3" s="3"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="U4" s="3"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="U5" s="3"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="U6" s="3"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="U7" s="3"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="U8" s="3"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="U9" s="3"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="U10" s="3"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="U11" s="3"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="U12" s="3"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="U13" s="3"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="U14" s="3"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="U15" s="3"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="U16" s="3"/>
-    </row>
-    <row r="17" spans="11:21" x14ac:dyDescent="0.25">
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="U17" s="3"/>
-    </row>
-    <row r="18" spans="11:21" x14ac:dyDescent="0.25">
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="U18" s="3"/>
-    </row>
-    <row r="19" spans="11:21" x14ac:dyDescent="0.25">
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="U19" s="3"/>
-    </row>
-    <row r="20" spans="11:21" x14ac:dyDescent="0.25">
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="U20" s="3"/>
-    </row>
-    <row r="21" spans="11:21" x14ac:dyDescent="0.25">
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="U21" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>